<commit_message>
Fixed Excel Reporter for Parallel execution
</commit_message>
<xml_diff>
--- a/ExcelReports/EcommerceTestResults.xlsx
+++ b/ExcelReports/EcommerceTestResults.xlsx
@@ -6,13 +6,13 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginTestClassResults" r:id="rId3" sheetId="1"/>
+    <sheet name="ValidationResults" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="9">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -27,6 +27,15 @@
   </si>
   <si>
     <t>testValidLogin</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>TC-TESTVALIDLOGIN2</t>
+  </si>
+  <si>
+    <t>testValidLogin2</t>
   </si>
   <si>
     <t>FAIL</t>
@@ -74,7 +83,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -102,6 +111,94 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed Unwanted Apache POI logs
</commit_message>
<xml_diff>
--- a/ExcelReports/EcommerceTestResults.xlsx
+++ b/ExcelReports/EcommerceTestResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>testValidLogin2</t>
-  </si>
-  <si>
-    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -83,7 +80,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -119,84 +116,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s" s="0">
         <v>5</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s" s="0">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s" s="0">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enhanced Extent reports with Emojies
</commit_message>
<xml_diff>
--- a/ExcelReports/EcommerceTestResults.xlsx
+++ b/ExcelReports/EcommerceTestResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>testValidLogin2</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -80,7 +83,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -116,7 +119,18 @@
         <v>7</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>5</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
latest Chance on test
</commit_message>
<xml_diff>
--- a/ExcelReports/EcommerceTestResults.xlsx
+++ b/ExcelReports/EcommerceTestResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -38,7 +38,10 @@
     <t>testValidLogin2</t>
   </si>
   <si>
-    <t>FAIL</t>
+    <t>TC-TESTVALIDLOGIN3</t>
+  </si>
+  <si>
+    <t>testValidLogin3</t>
   </si>
 </sst>
 </file>
@@ -83,7 +86,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -119,18 +122,40 @@
         <v>7</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
         <v>8</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Excel Report for group execution
</commit_message>
<xml_diff>
--- a/ExcelReports/EcommerceTestResults.xlsx
+++ b/ExcelReports/EcommerceTestResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -23,25 +23,16 @@
     <t>Status</t>
   </si>
   <si>
-    <t>TC-TESTVALIDLOGIN</t>
-  </si>
-  <si>
-    <t>testValidLogin</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>TC-TESTVALIDLOGIN2</t>
-  </si>
-  <si>
-    <t>testValidLogin2</t>
-  </si>
-  <si>
     <t>TC-TESTVALIDLOGIN3</t>
   </si>
   <si>
     <t>testValidLogin3</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -86,7 +77,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -116,21 +107,21 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>5</v>
@@ -138,24 +129,35 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented Trace Viewer for Testing Artifacts
</commit_message>
<xml_diff>
--- a/ExcelReports/EcommerceTestResults.xlsx
+++ b/ExcelReports/EcommerceTestResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -23,16 +23,25 @@
     <t>Status</t>
   </si>
   <si>
-    <t>TC-TESTVALIDLOGIN3</t>
+    <t>TC-TESTS.LOGINTEST2.TESTVALIDLOGIN3 [3.0, SECRET_SAUCE, TESTCASE]</t>
   </si>
   <si>
     <t>testValidLogin3</t>
   </si>
   <si>
-    <t>SKIP</t>
+    <t>PASS</t>
   </si>
   <si>
-    <t>FAIL</t>
+    <t>TC-TESTS.LOGINTEST.TESTVALIDLOGIN [3.0, SECRET_SAUCE, TESTCASE]</t>
+  </si>
+  <si>
+    <t>testValidLogin</t>
+  </si>
+  <si>
+    <t>TC-TESTS.LOGINTEST2.TESTVALIDLOGIN3 [4.0, SECRET_SAUCE, TESTCASE]</t>
+  </si>
+  <si>
+    <t>TC-TESTS.LOGINTEST2.TESTVALIDLOGIN3 [5.0, SECRET_SAUCE, TESTCASE]</t>
   </si>
 </sst>
 </file>
@@ -77,7 +86,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -107,18 +116,18 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s" s="0">
         <v>4</v>
@@ -129,35 +138,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s" s="0">
         <v>4</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s" s="0">
         <v>5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>